<commit_message>
Version 2.0 with admin and MongoDB
</commit_message>
<xml_diff>
--- a/prenursery_scores.xlsx
+++ b/prenursery_scores.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Serial Number</t>
   </si>
@@ -25,28 +25,25 @@
     <t>MATH Exam</t>
   </si>
   <si>
-    <t>COMPUTER CA</t>
-  </si>
-  <si>
-    <t>COMPUTER Exam</t>
-  </si>
-  <si>
-    <t>FRENCH CA</t>
-  </si>
-  <si>
-    <t>FRENCH Exam</t>
-  </si>
-  <si>
-    <t>UNIVERT CA</t>
-  </si>
-  <si>
-    <t>UNIVERT Exam</t>
-  </si>
-  <si>
-    <t>FAVOUR EMMANUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HANNAH </t>
+    <t>GRACE CA</t>
+  </si>
+  <si>
+    <t>GRACE Exam</t>
+  </si>
+  <si>
+    <t>AHHBOJ CA</t>
+  </si>
+  <si>
+    <t>AHHBOJ Exam</t>
+  </si>
+  <si>
+    <t>JLBO CA</t>
+  </si>
+  <si>
+    <t>JLBO Exam</t>
+  </si>
+  <si>
+    <t>HOUR</t>
   </si>
 </sst>
 </file>
@@ -427,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="15" customWidth="1"/>
@@ -476,51 +473,25 @@
         <v>13</v>
       </c>
       <c r="D2">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>19</v>
+      </c>
+      <c r="F2">
         <v>60</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>11</v>
       </c>
-      <c r="F2">
-        <v>19</v>
-      </c>
-      <c r="G2">
-        <v>15</v>
-      </c>
       <c r="H2">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I2">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>34</v>
-      </c>
-      <c r="D3">
-        <v>58</v>
-      </c>
-      <c r="E3">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>11</v>
-      </c>
-      <c r="G3">
-        <v>33</v>
-      </c>
-      <c r="H3">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>